<commit_message>
Daily Satellite Data Update
</commit_message>
<xml_diff>
--- a/Prelety.xlsx
+++ b/Prelety.xlsx
@@ -79,67 +79,67 @@
     <t>28.12.2025</t>
   </si>
   <si>
-    <t>00:38</t>
+    <t>00:37</t>
   </si>
   <si>
     <t>05:49</t>
   </si>
   <si>
-    <t>05:37</t>
+    <t>05:36</t>
   </si>
   <si>
     <t>09:02</t>
   </si>
   <si>
-    <t>10:42</t>
-  </si>
-  <si>
-    <t>10:35</t>
-  </si>
-  <si>
-    <t>05:48:39</t>
-  </si>
-  <si>
-    <t>06:15:39</t>
-  </si>
-  <si>
-    <t>05:40:50</t>
-  </si>
-  <si>
-    <t>05:52:50</t>
-  </si>
-  <si>
-    <t>06:18:05</t>
-  </si>
-  <si>
-    <t>05:43:19</t>
-  </si>
-  <si>
-    <t>05:53:09</t>
-  </si>
-  <si>
-    <t>06:21:00</t>
-  </si>
-  <si>
-    <t>05:46:07</t>
-  </si>
-  <si>
-    <t>05:53:28</t>
-  </si>
-  <si>
-    <t>06:23:54</t>
-  </si>
-  <si>
-    <t>05:48:56</t>
-  </si>
-  <si>
-    <t>05:57:41</t>
-  </si>
-  <si>
-    <t>06:26:21</t>
-  </si>
-  <si>
-    <t>05:51:25</t>
+    <t>10:43</t>
+  </si>
+  <si>
+    <t>10:36</t>
+  </si>
+  <si>
+    <t>05:48:36</t>
+  </si>
+  <si>
+    <t>06:15:33</t>
+  </si>
+  <si>
+    <t>05:40:42</t>
+  </si>
+  <si>
+    <t>05:52:49</t>
+  </si>
+  <si>
+    <t>06:18:00</t>
+  </si>
+  <si>
+    <t>05:43:12</t>
+  </si>
+  <si>
+    <t>05:53:07</t>
+  </si>
+  <si>
+    <t>06:20:54</t>
+  </si>
+  <si>
+    <t>05:45:59</t>
+  </si>
+  <si>
+    <t>05:53:26</t>
+  </si>
+  <si>
+    <t>06:23:49</t>
+  </si>
+  <si>
+    <t>05:48:48</t>
+  </si>
+  <si>
+    <t>05:57:38</t>
+  </si>
+  <si>
+    <t>06:26:16</t>
+  </si>
+  <si>
+    <t>05:51:18</t>
   </si>
   <si>
     <t>-</t>
@@ -185,7 +185,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,19 +212,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6697CD"/>
+        <fgColor rgb="FF5E92CB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF0707F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB2CBE6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -301,9 +295,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -804,16 +795,16 @@
         <v>44</v>
       </c>
       <c r="O2" s="6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="P2" s="7">
         <v>0</v>
       </c>
       <c r="Q2" s="8">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="R2" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -859,11 +850,11 @@
       <c r="N3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="9">
-        <v>53</v>
-      </c>
-      <c r="P3" s="10">
-        <v>53</v>
+      <c r="O3" s="6">
+        <v>3</v>
+      </c>
+      <c r="P3" s="8">
+        <v>3</v>
       </c>
       <c r="Q3" s="7">
         <v>0</v>
@@ -918,7 +909,7 @@
       <c r="O4" s="9">
         <v>90</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="10">
         <v>88</v>
       </c>
       <c r="Q4" s="7">

</xml_diff>